<commit_message>
2020/03/02 revise to 2020 by Kishiba
</commit_message>
<xml_diff>
--- a/win10_en.xlsx
+++ b/win10_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sumiya/Desktop/Work/2020/02/fresta/textdata-2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E749BE-26F3-B948-B24B-77EEF2772954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B479A127-0E14-4F77-B035-E5F39D46E2D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26880" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -239,9 +239,6 @@
     <t>Install required programs</t>
   </si>
   <si>
-    <t>FRESTA-TEXT-2019 Win10en chap.2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Copy the installation files in numbered USB flash drive to your PC. Here, you will install Microsoft Office and Google Chrome on your PC.
 &lt;ul&gt;&lt;li&gt;&lt;a href="#copy"&gt;Copy the files in the USB flash drive to your PC&lt;/a&gt;
 &lt;/li&gt;
@@ -310,12 +307,6 @@
   </si>
   <si>
     <t>&lt;h2&gt;&lt;a name="office"&gt;&lt;/a&gt;Install Microsoft Office&lt;/h2&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If Office2016 has already been installed on your PC, you can skip this section and &lt;a href="#chrome"&gt;proceed to step [10]&lt;/a&gt;
-. If you have Office2013 in your PC, you may install Office2016 on your PC.
-Double-click the copied &amp;quot;setup2019-win10en&amp;quot; folder on your desktop to open it. Then double-click the &amp;quot;office2016win-en&amp;quot; in the &amp;quot;windows-en&amp;quot; window. When you find the &amp;quot;install&amp;quot; item in the folder, double-click to start the installation.
-  </t>
   </si>
   <si>
     <t>win10-2-06.svg</t>
@@ -925,12 +916,23 @@
     <t>FRESTA-TEXT-2020 Win10</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t xml:space="preserve">If Office2016 has already been installed on your PC, you can skip this section and &lt;a href="#chrome"&gt;proceed to step [10]&lt;/a&gt;
+. If you have Office2013 in your PC, you may install Office2016 on your PC.
+Double-click the copied &amp;quot;setup2020-win10en&amp;quot; folder on your desktop to open it. Then double-click the &amp;quot;officepropluswin-en&amp;quot; in the &amp;quot;windows-en&amp;quot; window. When you find the &amp;quot;install&amp;quot; item in the folder, double-click to start the installation.
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2020 Win10en chap.2</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -946,12 +948,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -966,9 +974,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1311,19 +1322,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1331,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1339,20 +1350,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="75">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1361,7 +1372,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="60">
+    <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1385,17 +1396,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1403,7 +1416,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1411,7 +1424,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1419,7 +1432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="60">
+    <row r="5" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1433,7 +1446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30">
+    <row r="6" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1447,7 +1460,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45">
+    <row r="7" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1461,7 +1474,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
+    <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1475,7 +1488,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30">
+    <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1489,7 +1502,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="90">
+    <row r="10" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1503,7 +1516,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30">
+    <row r="11" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1517,7 +1530,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="60">
+    <row r="12" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1531,7 +1544,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="60">
+    <row r="13" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1545,7 +1558,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="90">
+    <row r="14" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1559,7 +1572,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30">
+    <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1573,7 +1586,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30">
+    <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1587,7 +1600,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="105">
+    <row r="17" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1601,7 +1614,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30">
+    <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1625,17 +1638,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1643,7 +1658,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1651,7 +1666,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1659,7 +1674,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1667,7 +1682,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="120">
+    <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1681,7 +1696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="90">
+    <row r="7" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1695,7 +1710,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="195">
+    <row r="8" spans="1:4" ht="182" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1709,7 +1724,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="75">
+    <row r="9" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1723,7 +1738,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="165">
+    <row r="10" spans="1:4" ht="169" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1747,17 +1762,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1765,7 +1782,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1773,7 +1790,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1781,219 +1798,220 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="130" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="150">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15">
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="195" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="210">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15">
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="30">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>58</v>
       </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="30">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>60</v>
       </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="30">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>62</v>
       </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="60">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>64</v>
       </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="45">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
         <v>66</v>
       </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15">
-      <c r="B15" s="1" t="s">
+    <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="90">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="45">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1" t="s">
+    <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="30">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
       </c>
       <c r="D19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15">
-      <c r="B20" s="1" t="s">
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="1" t="s">
+    <row r="22" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="75">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2001,33 +2019,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2035,152 +2055,152 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="143" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="60">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="150">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="75">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="105">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="60">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="11" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="90">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="12" spans="1:4" ht="78" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="90">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="D13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="75">
-      <c r="A14" t="s">
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="182" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="210">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2195,31 +2215,31 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2227,251 +2247,251 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="143" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="165">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15">
-      <c r="B7" s="1" t="s">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="11" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="90">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15">
-      <c r="B13" s="1" t="s">
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="60">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="105">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    <row r="17" spans="1:4" ht="78" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="75">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1" t="s">
+    <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="90">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="120">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15">
-      <c r="B20" s="1" t="s">
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="60">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="1" t="s">
+    <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="1" t="s">
+    <row r="23" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="60">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="1" t="s">
+    <row r="24" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="45">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2484,33 +2504,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2518,513 +2540,513 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="208" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="225">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15">
-      <c r="B7" s="1" t="s">
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="60">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="60">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15">
-      <c r="B11" s="1" t="s">
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="15" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="45">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C17" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="30">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="D17" t="s">
         <v>159</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="90">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    <row r="20" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="60">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15">
-      <c r="B21" s="1" t="s">
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="45">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="1" t="s">
+    <row r="24" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="60">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="1" t="s">
+    <row r="25" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="1" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15">
-      <c r="B26" s="1" t="s">
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15">
-      <c r="A27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="60">
-      <c r="A28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="1" t="s">
+    <row r="29" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30">
-      <c r="A29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="1" t="s">
+    <row r="30" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="60">
-      <c r="A30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="1" t="s">
+    <row r="31" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="1" t="s">
+    <row r="32" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30">
-      <c r="A32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="1" t="s">
+    <row r="33" spans="1:4" ht="234" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="240">
-      <c r="A33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="1" t="s">
+    <row r="34" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="105">
-      <c r="A34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="1" t="s">
+    <row r="35" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="45">
-      <c r="A35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" s="1" t="s">
+    <row r="36" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="45">
-      <c r="A36" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="1" t="s">
+    <row r="37" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="75">
-      <c r="A37" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="1" t="s">
+    <row r="38" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="75">
-      <c r="A38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" s="1" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" t="s">
+    </row>
+    <row r="40" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="15">
-      <c r="B39" s="1" t="s">
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="143" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="30">
-      <c r="A40" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C40" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="120">
-      <c r="A41" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="C41" t="s">
         <v>12</v>
       </c>
       <c r="D41" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="45">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C42" t="s">
         <v>12</v>
       </c>
       <c r="D42" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="135">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="117" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C43" t="s">
         <v>12</v>
       </c>
       <c r="D43" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="105">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C44" t="s">
         <v>12</v>
       </c>
       <c r="D44" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3039,23 +3061,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3063,44 +3085,44 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15">
-      <c r="B6" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="208" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15">
-      <c r="B7" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="210">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
fix win10_en sheet title
</commit_message>
<xml_diff>
--- a/win10_en.xlsx
+++ b/win10_en.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750028F5-1247-4F62-8F8E-004827B7A207}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274F280E-BE12-4422-99EA-3D9C687C9364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40125" yWindow="195" windowWidth="13500" windowHeight="8265" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1970" yWindow="1980" windowWidth="13500" windowHeight="8260" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
-    <sheet name="ch0 " sheetId="9" r:id="rId2"/>
+    <sheet name="ch0" sheetId="9" r:id="rId2"/>
     <sheet name="ch1" sheetId="3" r:id="rId3"/>
     <sheet name="ch2" sheetId="4" r:id="rId4"/>
     <sheet name="ch3" sheetId="5" r:id="rId5"/>
@@ -1472,7 +1472,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1546,13 +1546,13 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="19.5" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6328125" customWidth="1" phonetic="1"/>
-    <col min="2" max="2" width="100.6328125" style="1" customWidth="1" phonetic="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.6328125" customWidth="1" phonetic="1"/>
     <col min="4" max="4" width="20.6328125" customWidth="1" phonetic="1"/>
     <col min="5" max="16384" width="8.81640625" phonetic="1"/>
@@ -1562,7 +1562,7 @@
       <c r="A1" t="s" ph="1">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s" ph="1">
+      <c r="B1" s="1" t="s">
         <v>172</v>
       </c>
     </row>
@@ -1570,7 +1570,7 @@
       <c r="A2" t="s" ph="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s" ph="1">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1578,7 +1578,7 @@
       <c r="A3" t="s" ph="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s" ph="1">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1586,15 +1586,15 @@
       <c r="A4" t="s" ph="1">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s" ph="1">
+      <c r="B4" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="52" ph="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s" ph="1">
+      <c r="B6" s="1" t="s">
         <v>174</v>
       </c>
       <c r="C6" t="s" ph="1">
@@ -1604,11 +1604,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s" ph="1">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s" ph="1">
@@ -1618,11 +1618,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s" ph="1">
+      <c r="B8" s="1" t="s">
         <v>175</v>
       </c>
       <c r="C8" t="s" ph="1">
@@ -1632,11 +1632,11 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s" ph="1">
+      <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C9" t="s" ph="1">
@@ -1646,19 +1646,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s" ph="1">
+    <row r="10" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
         <v>177</v>
       </c>
       <c r="D10" t="s" ph="1">
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s" ph="1">
+      <c r="B11" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C11" t="s" ph="1">
@@ -1668,11 +1668,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B12" s="1" t="s" ph="1">
+      <c r="B12" s="1" t="s">
         <v>180</v>
       </c>
       <c r="C12" t="s" ph="1">
@@ -1682,19 +1682,19 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s" ph="1">
+    <row r="13" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>182</v>
       </c>
       <c r="D13" t="s" ph="1">
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B14" s="1" t="s" ph="1">
+      <c r="B14" s="1" t="s">
         <v>184</v>
       </c>
       <c r="C14" t="s" ph="1">
@@ -1704,11 +1704,11 @@
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="52" ph="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B15" s="1" t="s" ph="1">
+      <c r="B15" s="1" t="s">
         <v>186</v>
       </c>
       <c r="C15" t="s" ph="1">
@@ -1718,11 +1718,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="52" ph="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B16" s="1" t="s" ph="1">
+      <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s" ph="1">
@@ -1733,18 +1733,18 @@
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s" ph="1">
+      <c r="B17" s="1" t="s">
         <v>187</v>
       </c>
       <c r="D17" t="s" ph="1">
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B18" s="1" t="s" ph="1">
+      <c r="B18" s="1" t="s">
         <v>189</v>
       </c>
       <c r="C18" t="s" ph="1">
@@ -1754,11 +1754,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B19" s="1" t="s" ph="1">
+      <c r="B19" s="1" t="s">
         <v>191</v>
       </c>
       <c r="C19" t="s" ph="1">
@@ -1768,19 +1768,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s" ph="1">
+    <row r="20" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>192</v>
       </c>
       <c r="D20" t="s" ph="1">
         <v>193</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B21" s="1" t="s" ph="1">
+      <c r="B21" s="1" t="s">
         <v>194</v>
       </c>
       <c r="C21" t="s" ph="1">
@@ -1790,11 +1790,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="136.5" ph="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="91" ph="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B22" s="1" t="s" ph="1">
+      <c r="B22" s="1" t="s">
         <v>196</v>
       </c>
       <c r="C22" t="s" ph="1">
@@ -1804,11 +1804,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B23" s="1" t="s" ph="1">
+      <c r="B23" s="1" t="s">
         <v>198</v>
       </c>
       <c r="C23" t="s" ph="1">
@@ -1829,8 +1829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2211,8 +2211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3318,7 +3318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix win10e add some pics
</commit_message>
<xml_diff>
--- a/win10_en.xlsx
+++ b/win10_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97D3DA1-088E-47DF-A83E-74F7732ADDC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67A5260-E60D-4699-9511-0E50C7B87235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27120" yWindow="1035" windowWidth="16890" windowHeight="12270" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37545" yWindow="1725" windowWidth="16890" windowHeight="10155" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="225">
   <si>
     <t>header1</t>
   </si>
@@ -55,11 +55,6 @@
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t xml:space="preserve">You are going to prepare your PC for your study life at Hiroshima University during this lecture. Here is the list of what you are going to do today.
-&lt;ol&gt; &lt;/ol&gt;
-  </t>
   </si>
   <si>
     <t>fresta</t>
@@ -147,9 +142,6 @@
     <t>&lt;h2&gt;&lt;a name="chrome"&gt;&lt;/a&gt;Install Google Chrome&lt;/h2&gt;</t>
   </si>
   <si>
-    <t>win10-2-10.svg</t>
-  </si>
-  <si>
     <t xml:space="preserve">The installation will be completed in a minute!
 &lt;p class="spl"&gt;* You may realize that Microsoft Edge, as the default browser, has already been in Windows 10. But there are some web pages which cannot be displayed successfully by Microsoft Edge. In that case, you can use Google Chrome as the secondary browser.&lt;/p&gt;
   </t>
@@ -174,11 +166,6 @@
   </si>
   <si>
     <t>win10-4-02.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Now you can see the list of Wi-Fi AP (access points) which your PC can detect. Choose Wi-Fi AP named like &amp;quot;HU-CUPxx&amp;quot;. Here, each x represents a number. The two-digit number is different from the area in the campus. For examples, you will find &amp;quot;HU-CUP30&amp;quot; near School of Integrated Arts and Sciences, &amp;quot;HU-CUP40&amp;quot; in Kasumi campus, or &amp;quot;HU-CUP50&amp;quot; in Higashisneda campus.
-&lt;p class="spl"&gt;&amp;amp;ast; If your PC could not detect Wi-Fi AP named &amp;quot;HU-CUPxx&amp;quot; in classroom, it possiblly does not meet system requirement, it should support 5GHz Wi-Fi. Please contact IMC staff.&lt;/p&gt;
-  </t>
   </si>
   <si>
     <t>win10-4-03.svg</t>
@@ -966,12 +953,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">The window says, &amp;quot;We&amp;apos;ll be done in just a moment.&amp;quot; Wait &lt;it&gt;a few&lt;/it&gt; minutes.
-Click &amp;quot;Finished&amp;quot;.
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">Input HIRODAI mailaddress（b20xxxxx@hiroshima-u.ac.jp）and click &amp;quot;Next&amp;quot;.
   </t>
     <phoneticPr fontId="1"/>
@@ -1004,14 +985,49 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t xml:space="preserve">For your better PC life, IMC holds F3S, First Three Steps, Workshops. 
+In the workshop, you may get some useful knowledge or technique to use your PC. Join us if you are interested in the themes. 
+&lt;ul&gt;&lt;li&gt;&lt;a href="https://f3s.riise.hiroshima-u.ac.jp"&gt;https://f3s.riise.hiroshima-u.ac.jp&lt;/a&gt;
+ &lt;/li&gt;
+&lt;/ul&gt;
+ </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">You are going to prepare your PC for your study life at Hiroshima University during this lecture. Here is the list of what you are going to do at this workshop.
+&lt;ol&gt; &lt;/ol&gt;
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Now you can see the list of Wi-Fi AP (access points) which your PC can detect. Choose Wi-Fi AP named like &amp;quot;HU-CUPxx&amp;quot;. Here, each x represents a number. The two-digit number is different from the area in the campus. For examples, you will find &amp;quot;HU-CUP30&amp;quot; near School of Integrated Arts and Sciences, &amp;quot;HU-CUP40&amp;quot; in Kasumi campus, or &amp;quot;HU-CUP50&amp;quot; in Higashisneda campus.
+&lt;p class="spl"&gt;&amp;ast; If your PC could not detect Wi-Fi AP named &amp;quot;HU-CUPxx&amp;quot; in classroom, it possiblly does not meet system requirement, it should support 5GHz Wi-Fi. Please contact IMC staff.&lt;/p&gt;
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-4-01.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-2-41.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The window says, &amp;quot;We&amp;apos;ll be done in just a moment.&amp;quot; Wait &lt;it&gt;a few&lt;/it&gt; minutes.
+Click &amp;quot;Finish&amp;quot;.
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t xml:space="preserve">If you are in trouble when you use your PC, don&amp;apos;t hesitate to make a inquiry to IMC.
 &lt;dl&gt;&lt;dt&gt;At IMC: &lt;/dt&gt;
 &lt;dt&gt; &lt;/dt&gt;
-&lt;dd&gt;Startup workshop (Apr.4-8, for detail, see below URL)&lt;/dd&gt;
+&lt;dd&gt;&amp;ast;Startup workshop (Apr.4-8, for detail, see below URL)&lt;/dd&gt;
 &lt;dd&gt;&lt;a href="https://info.pre-entrance.hiroshima-u.ac.jp/"&gt;https://info.pre-entrance.hiroshima-u.ac.jp/&lt;/a&gt;&lt;/dd&gt;
-&lt;dd&gt;Special QA Support (Apr.4-5, 9:00-17:00)&lt;/dd&gt;
-&lt;dd&gt;IMC mail building&lt;/dd&gt;
-&lt;dd&gt;Support Desks (9:00-16:30 Weekday)&lt;/dd&gt;
+&lt;dd&gt;&amp;ast;Special QA Support (Apr.4-5, 9:00-17:00)&lt;/dd&gt;
+&lt;dd&gt;IMC main building&lt;/dd&gt;
+&lt;dd&gt;&amp;ast;Support Desks (9:00-16:30 Weekday)&lt;/dd&gt;
 &lt;dd&gt;IMC main building, IMC east branch in East Library, IMC service desk in West Library and Central Library, IMC Kasumi branch&lt;/dd&gt;
 &lt;dd&gt;&lt;a href="https://www.media.hiroshima-u.ac.jp/helpdesk"&gt;Access map&lt;/a&gt;&lt;/dd&gt;
 &lt;dt&gt;Online: &lt;/dt&gt;
@@ -1022,15 +1038,6 @@
 &lt;dt&gt; &lt;/dt&gt;
 &lt;dd&gt;&lt;a href="mailto:st-pc@ml.hiroshima-u.ac.jp"&gt;st-pc@ml.hiroshima-u.ac.jp&lt;/a&gt;
 &lt;/dd&gt; &lt;/dl&gt;
- </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">For your better PC life, IMC holds F3S, First Three Steps, Workshops. 
-In the workshop, you may get some useful knowledge or technique to use your PC. Join us if you are interested in the themes. 
-&lt;ul&gt;&lt;li&gt;&lt;a href="https://f3s.riise.hiroshima-u.ac.jp"&gt;https://f3s.riise.hiroshima-u.ac.jp&lt;/a&gt;
- &lt;/li&gt;
-&lt;/ul&gt;
  </t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1430,7 +1437,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1462,7 +1469,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -1470,7 +1477,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1484,7 +1491,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>219</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1496,6 +1503,7 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1503,8 +1511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0FC8B8-3740-45D4-A5FA-75052BCDA48C}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="19.5" x14ac:dyDescent="0.2"/>
@@ -1518,10 +1526,10 @@
   <sheetData>
     <row r="1" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s" ph="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1529,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1537,7 +1545,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1545,7 +1553,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52" ph="1" x14ac:dyDescent="0.2">
@@ -1553,7 +1561,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>5</v>
@@ -1567,13 +1575,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s" ph="1">
         <v>8</v>
       </c>
-      <c r="C7" t="s" ph="1">
+      <c r="D7" t="s" ph="1">
         <v>9</v>
-      </c>
-      <c r="D7" t="s" ph="1">
-        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1581,13 +1589,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
@@ -1595,21 +1603,21 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s" ph="1">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s" ph="1">
         <v>11</v>
-      </c>
-      <c r="C9" t="s" ph="1">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s" ph="1">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
@@ -1617,13 +1625,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C11" t="s" ph="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1631,21 +1639,21 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C12" t="s" ph="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
@@ -1653,13 +1661,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C14" t="s" ph="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52" ph="1" x14ac:dyDescent="0.2">
@@ -1667,13 +1675,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C15" t="s" ph="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="52" ph="1" x14ac:dyDescent="0.2">
@@ -1681,21 +1689,21 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s" ph="1">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s" ph="1">
         <v>15</v>
-      </c>
-      <c r="C16" t="s" ph="1">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s" ph="1">
-        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
@@ -1703,13 +1711,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C18" t="s" ph="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
@@ -1717,21 +1725,21 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C19" t="s" ph="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
@@ -1739,13 +1747,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C21" t="s" ph="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="91" ph="1" x14ac:dyDescent="0.2">
@@ -1753,13 +1761,13 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C22" t="s" ph="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
@@ -1767,13 +1775,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C23" t="s" ph="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1801,10 +1809,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1812,7 +1820,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1820,7 +1828,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1828,7 +1836,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -1836,7 +1844,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1850,13 +1858,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
         <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="182" x14ac:dyDescent="0.2">
@@ -1864,13 +1872,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -1878,13 +1886,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -1892,13 +1900,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1912,8 +1920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1926,10 +1934,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1937,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1945,7 +1953,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1953,12 +1961,12 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -1966,13 +1974,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -1980,13 +1988,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -1994,13 +2002,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2008,13 +2016,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>220</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2022,13 +2030,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2036,13 +2044,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2050,21 +2058,21 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -2078,13 +2086,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2111,10 +2119,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2122,7 +2130,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2130,7 +2138,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2138,7 +2146,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2146,7 +2154,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2157,7 +2165,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2165,13 +2173,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2179,13 +2187,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2193,13 +2201,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2207,13 +2215,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2221,18 +2229,18 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2240,13 +2248,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2254,13 +2262,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2268,13 +2276,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2282,13 +2290,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2296,13 +2304,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2310,13 +2318,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2331,7 +2339,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2344,10 +2352,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2355,7 +2363,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2363,7 +2371,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2371,7 +2379,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -2379,7 +2387,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2390,7 +2398,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="156" x14ac:dyDescent="0.2">
@@ -2398,18 +2406,18 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2417,37 +2425,37 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D12" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2455,13 +2463,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2469,18 +2477,18 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2488,21 +2496,21 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D18" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2510,13 +2518,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2524,13 +2532,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2538,13 +2546,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2552,13 +2560,13 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2566,13 +2574,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2600,10 +2608,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2611,7 +2619,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2619,7 +2627,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2627,7 +2635,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="208" x14ac:dyDescent="0.2">
@@ -2635,7 +2643,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2646,7 +2654,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2668,13 +2676,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2682,18 +2690,18 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2715,13 +2723,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2729,13 +2737,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2743,13 +2751,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2757,13 +2765,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2771,13 +2779,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2785,13 +2793,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2799,13 +2807,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2813,13 +2821,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2827,18 +2835,18 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2860,13 +2868,13 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2874,13 +2882,13 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2888,18 +2896,18 @@
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -2921,13 +2929,13 @@
         <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2935,13 +2943,13 @@
         <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2949,13 +2957,13 @@
         <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2963,13 +2971,13 @@
         <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2977,13 +2985,13 @@
         <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -2991,13 +2999,13 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3005,13 +3013,13 @@
         <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3019,13 +3027,13 @@
         <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3033,13 +3041,13 @@
         <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3047,13 +3055,13 @@
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3061,18 +3069,18 @@
         <v>5</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3080,7 +3088,7 @@
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -3094,13 +3102,13 @@
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3108,13 +3116,13 @@
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -3122,21 +3130,21 @@
         <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3144,13 +3152,13 @@
         <v>5</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3165,7 +3173,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3181,7 +3189,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3189,7 +3197,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3197,7 +3205,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3205,7 +3213,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -3216,7 +3224,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="260" x14ac:dyDescent="0.2">
@@ -3224,7 +3232,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -3235,7 +3243,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -3243,7 +3251,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
fix win10e info of support desk
</commit_message>
<xml_diff>
--- a/win10_en.xlsx
+++ b/win10_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67A5260-E60D-4699-9511-0E50C7B87235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90D19F5-C7C0-4FDD-B3BB-BB530E78EA3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37545" yWindow="1725" windowWidth="16890" windowHeight="10155" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36660" yWindow="2040" windowWidth="16890" windowHeight="10155" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -1023,11 +1023,11 @@
     <t xml:space="preserve">If you are in trouble when you use your PC, don&amp;apos;t hesitate to make a inquiry to IMC.
 &lt;dl&gt;&lt;dt&gt;At IMC: &lt;/dt&gt;
 &lt;dt&gt; &lt;/dt&gt;
-&lt;dd&gt;&amp;ast;Startup workshop (Apr.4-8, for detail, see below URL)&lt;/dd&gt;
+&lt;dd&gt;&amp;ast; Startup workshop (Apr.4-8, for detail, see below URL)&lt;/dd&gt;
 &lt;dd&gt;&lt;a href="https://info.pre-entrance.hiroshima-u.ac.jp/"&gt;https://info.pre-entrance.hiroshima-u.ac.jp/&lt;/a&gt;&lt;/dd&gt;
-&lt;dd&gt;&amp;ast;Special QA Support (Apr.4-5, 9:00-17:00)&lt;/dd&gt;
+&lt;dd&gt;&amp;ast; Special QA Support (Apr.4 12:30-17:00, Apr.5 9:00-17:00)&lt;/dd&gt;
 &lt;dd&gt;IMC main building&lt;/dd&gt;
-&lt;dd&gt;&amp;ast;Support Desks (9:00-16:30 Weekday)&lt;/dd&gt;
+&lt;dd&gt;&amp;ast; Support Desks (9:00-16:30 Weekday)&lt;/dd&gt;
 &lt;dd&gt;IMC main building, IMC east branch in East Library, IMC service desk in West Library and Central Library, IMC Kasumi branch&lt;/dd&gt;
 &lt;dd&gt;&lt;a href="https://www.media.hiroshima-u.ac.jp/helpdesk"&gt;Access map&lt;/a&gt;&lt;/dd&gt;
 &lt;dt&gt;Online: &lt;/dt&gt;
@@ -1920,7 +1920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2105,8 +2105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2338,8 +2338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3172,7 +3172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3263,5 +3263,6 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add template for English ver
</commit_message>
<xml_diff>
--- a/win10_en.xlsx
+++ b/win10_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6982CEB4-9848-470E-BE98-B31D6699C487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154123C4-46C0-4786-8177-70E89F75FD20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36495" yWindow="645" windowWidth="13425" windowHeight="10575" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36495" yWindow="645" windowWidth="13425" windowHeight="10575" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t/>
   </si>
   <si>
-    <t>fresta</t>
-  </si>
-  <si>
     <t>chartn</t>
   </si>
   <si>
@@ -1041,6 +1038,10 @@
   </si>
   <si>
     <t>win10-6-31.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>fresta_en</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1439,7 +1440,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1471,7 +1472,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -1479,7 +1480,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1493,7 +1494,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1513,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0FC8B8-3740-45D4-A5FA-75052BCDA48C}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="106" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="B1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="19.5" x14ac:dyDescent="0.2"/>
@@ -1528,10 +1529,10 @@
   <sheetData>
     <row r="1" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s" ph="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1539,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1547,7 +1548,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1555,7 +1556,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1563,7 +1564,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>5</v>
@@ -1577,13 +1578,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C7" t="s" ph="1">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s" ph="1">
         <v>7</v>
-      </c>
-      <c r="D7" t="s" ph="1">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
@@ -1591,13 +1592,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1605,21 +1606,21 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C9" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
@@ -1627,13 +1628,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C11" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1641,40 +1642,40 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C12" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C14" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1682,13 +1683,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C16" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1696,13 +1697,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C17" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1710,21 +1711,21 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C18" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1732,13 +1733,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C20" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52" ph="1" x14ac:dyDescent="0.2">
@@ -1746,21 +1747,21 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C21" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
@@ -1768,13 +1769,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C23" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="65" ph="1" x14ac:dyDescent="0.2">
@@ -1782,13 +1783,13 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C24" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1796,13 +1797,13 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C25" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -1816,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1830,10 +1831,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1841,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1849,7 +1850,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1857,7 +1858,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -1865,7 +1866,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1879,13 +1880,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="182" x14ac:dyDescent="0.2">
@@ -1893,13 +1894,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -1907,13 +1908,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -1921,13 +1922,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1941,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1955,10 +1956,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1966,7 +1967,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1974,7 +1975,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1982,12 +1983,12 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -1995,13 +1996,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -2009,13 +2010,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2023,13 +2024,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>31</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2037,13 +2038,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2051,13 +2052,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2065,13 +2066,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2079,21 +2080,21 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -2107,13 +2108,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2126,8 +2127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2140,10 +2141,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2151,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2159,7 +2160,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2167,7 +2168,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2175,7 +2176,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2186,7 +2187,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2194,13 +2195,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
         <v>46</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2208,13 +2209,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>48</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2222,13 +2223,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2236,13 +2237,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2250,18 +2251,18 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>52</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2269,13 +2270,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2283,13 +2284,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
         <v>55</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2297,13 +2298,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2311,13 +2312,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
         <v>58</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2325,13 +2326,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2339,13 +2340,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2359,8 +2360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2373,10 +2374,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2384,7 +2385,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2392,7 +2393,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2400,7 +2401,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -2408,7 +2409,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2419,7 +2420,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="156" x14ac:dyDescent="0.2">
@@ -2427,18 +2428,18 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2446,37 +2447,37 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2484,13 +2485,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2498,18 +2499,18 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
         <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2517,21 +2518,21 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2539,13 +2540,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2553,13 +2554,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2567,13 +2568,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2581,13 +2582,13 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2595,13 +2596,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2615,8 +2616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C35" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2629,10 +2630,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2640,7 +2641,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2648,7 +2649,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2656,7 +2657,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="208" x14ac:dyDescent="0.2">
@@ -2664,7 +2665,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2675,7 +2676,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2697,13 +2698,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>64</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2711,18 +2712,18 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>66</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2744,13 +2745,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>69</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2758,13 +2759,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
         <v>71</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2772,13 +2773,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2786,13 +2787,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2800,13 +2801,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
         <v>74</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2814,13 +2815,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
         <v>76</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>77</v>
-      </c>
-      <c r="D18" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2828,13 +2829,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2842,13 +2843,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
         <v>80</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2856,18 +2857,18 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
         <v>82</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2889,13 +2890,13 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
         <v>85</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2903,13 +2904,13 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2917,18 +2918,18 @@
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
         <v>88</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -2950,13 +2951,13 @@
         <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
         <v>91</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2964,13 +2965,13 @@
         <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
         <v>93</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2978,13 +2979,13 @@
         <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
         <v>95</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2992,13 +2993,13 @@
         <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
         <v>97</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3006,13 +3007,13 @@
         <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
         <v>99</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="195" x14ac:dyDescent="0.2">
@@ -3020,13 +3021,13 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3034,7 +3035,7 @@
         <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
@@ -3045,7 +3046,7 @@
         <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
@@ -3056,13 +3057,13 @@
         <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3070,23 +3071,23 @@
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
         <v>219</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3094,7 +3095,7 @@
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -3108,13 +3109,13 @@
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3122,13 +3123,13 @@
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
         <v>104</v>
-      </c>
-      <c r="C43" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -3136,21 +3137,21 @@
         <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
         <v>106</v>
-      </c>
-      <c r="C44" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3158,13 +3159,13 @@
         <v>5</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
         <v>108</v>
-      </c>
-      <c r="C46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -3178,8 +3179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3195,7 +3196,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3203,7 +3204,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3211,7 +3212,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3219,7 +3220,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -3230,7 +3231,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="260" x14ac:dyDescent="0.2">
@@ -3238,7 +3239,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -3249,7 +3250,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -3257,7 +3258,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
fix mac/win8.1 account B20x
</commit_message>
<xml_diff>
--- a/win10_en.xlsx
+++ b/win10_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E9B9DF-8A1B-4A80-9DFB-F29B301172AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254D9D5B-1835-48F8-9406-D765DD3DDD57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29970" yWindow="2535" windowWidth="13425" windowHeight="10575" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27330" yWindow="2490" windowWidth="13425" windowHeight="10575" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -393,9 +393,6 @@
   </t>
   </si>
   <si>
-    <t>win10-6-15.svg</t>
-  </si>
-  <si>
     <t xml:space="preserve">For your first login, this page will be shown. Click &amp;quot;Close&amp;quot;.
   </t>
   </si>
@@ -634,10 +631,6 @@
   </si>
   <si>
     <t>Initial setting of your PC</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>If you are going to turn on your PC for the first time, follow this chapter to see your Desktop in your PC.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -820,10 +813,6 @@
   </si>
   <si>
     <t>Click &amp;quot;Accept&amp;quot; to accept Windows 10 License Agreement.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Microsoft Teams will run automatically. Click x at left up in the window to close the application for now.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1047,6 +1036,18 @@
   </si>
   <si>
     <t>win10-6-35.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If you turn on your PC for the first time, follow this chapter to see your Desktop in your PC.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Microsoft Teams will run automatically. Click x at right up in the window to close the application for now.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-6-15e.svg</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1477,7 +1478,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -1485,7 +1486,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1499,7 +1500,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1519,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0FC8B8-3740-45D4-A5FA-75052BCDA48C}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="106" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="B15" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="19.5" x14ac:dyDescent="0.2"/>
@@ -1537,7 +1538,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>151</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1545,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1561,7 +1562,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1569,7 +1570,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>5</v>
@@ -1583,7 +1584,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>7</v>
@@ -1597,13 +1598,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
@@ -1611,7 +1612,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>7</v>
@@ -1622,10 +1623,10 @@
     </row>
     <row r="10" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
@@ -1633,7 +1634,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>7</v>
@@ -1647,40 +1648,40 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1688,13 +1689,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1702,7 +1703,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
@@ -1716,7 +1717,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
@@ -1727,10 +1728,10 @@
     </row>
     <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52" ph="1" x14ac:dyDescent="0.2">
@@ -1738,13 +1739,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1752,7 +1753,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
@@ -1763,10 +1764,10 @@
     </row>
     <row r="22" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
@@ -1774,13 +1775,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="65" ph="1" x14ac:dyDescent="0.2">
@@ -1788,13 +1789,13 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1802,13 +1803,13 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>186</v>
+        <v>225</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -1822,8 +1823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1839,7 +1840,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1863,7 +1864,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -1899,7 +1900,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -1927,7 +1928,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -1947,8 +1948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1988,12 +1989,12 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2001,7 +2002,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -2015,7 +2016,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -2043,7 +2044,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -2085,7 +2086,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -2119,7 +2120,7 @@
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2132,8 +2133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2173,7 +2174,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2181,7 +2182,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2242,13 +2243,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2275,13 +2276,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2303,7 +2304,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -2331,13 +2332,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2345,13 +2346,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2365,8 +2366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2382,7 +2383,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2406,7 +2407,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -2414,7 +2415,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2433,13 +2434,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2452,37 +2453,37 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2490,13 +2491,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2515,7 +2516,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2523,21 +2524,21 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2545,13 +2546,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2559,13 +2560,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2573,13 +2574,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2587,13 +2588,13 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2601,13 +2602,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2621,8 +2622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C35" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2662,7 +2663,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="208" x14ac:dyDescent="0.2">
@@ -2778,13 +2779,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2792,7 +2793,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -2834,7 +2835,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -2848,7 +2849,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -2909,7 +2910,7 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -3004,7 +3005,7 @@
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3012,13 +3013,13 @@
         <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
         <v>98</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="195" x14ac:dyDescent="0.2">
@@ -3026,13 +3027,13 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3040,13 +3041,13 @@
         <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3054,13 +3055,13 @@
         <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3068,13 +3069,13 @@
         <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3082,26 +3083,26 @@
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D39" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3109,7 +3110,7 @@
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -3123,13 +3124,13 @@
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3137,13 +3138,13 @@
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -3151,21 +3152,21 @@
         <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3173,13 +3174,13 @@
         <v>5</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3210,7 +3211,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3226,7 +3227,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3234,7 +3235,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -3245,7 +3246,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="260" x14ac:dyDescent="0.2">
@@ -3253,7 +3254,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -3264,7 +3265,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -3272,7 +3273,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
win10e fix index start button
</commit_message>
<xml_diff>
--- a/win10_en.xlsx
+++ b/win10_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254D9D5B-1835-48F8-9406-D765DD3DDD57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE68AC6-6318-47CB-9D91-710C78EC4760}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27330" yWindow="2490" windowWidth="13425" windowHeight="10575" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>template</t>
-  </si>
-  <si>
-    <t>index</t>
   </si>
   <si>
     <t>title</t>
@@ -1048,6 +1045,10 @@
   </si>
   <si>
     <t>win10-6-15e.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>index_en</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1445,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1470,43 +1471,43 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1535,10 +1536,10 @@
   <sheetData>
     <row r="1" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s" ph="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1546,7 +1547,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1554,262 +1555,262 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s" ph="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s" ph="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C6" t="s" ph="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s" ph="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s" ph="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C7" t="s" ph="1">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s" ph="1">
         <v>7</v>
-      </c>
-      <c r="D7" t="s" ph="1">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s" ph="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s" ph="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C9" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s" ph="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C11" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s" ph="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C12" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C14" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s" ph="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C16" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s" ph="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C17" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s" ph="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C18" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52" ph="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s" ph="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C20" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s" ph="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C21" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s" ph="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C23" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="65" ph="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s" ph="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C24" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s" ph="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C25" t="s" ph="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -1837,10 +1838,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1848,7 +1849,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1856,85 +1857,85 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="182" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="143" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1962,10 +1963,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1973,7 +1974,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1981,146 +1982,146 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="143" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>31</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="182" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2147,10 +2148,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2158,7 +2159,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2166,193 +2167,193 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>46</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>48</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>52</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
         <v>55</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>58</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2380,10 +2381,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2391,7 +2392,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2399,216 +2400,216 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="117" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="156" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
         <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2622,7 +2623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
+    <sheetView topLeftCell="C31" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -2636,10 +2637,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2647,7 +2648,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2655,532 +2656,532 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="208" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>64</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>66</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>69</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>71</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>74</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
         <v>76</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>77</v>
-      </c>
-      <c r="D18" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
         <v>81</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
         <v>84</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>87</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
         <v>90</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
         <v>92</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
         <v>94</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
         <v>97</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="195" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
         <v>199</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="143" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
         <v>102</v>
-      </c>
-      <c r="C43" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="117" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
         <v>104</v>
-      </c>
-      <c r="C44" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
         <v>106</v>
-      </c>
-      <c r="C46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3211,7 +3212,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3219,67 +3220,67 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="260" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win10e fix page transition button
</commit_message>
<xml_diff>
--- a/win10_en.xlsx
+++ b/win10_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE68AC6-6318-47CB-9D91-710C78EC4760}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B17735D-A313-4CF2-A8BF-CA8A1A6C5F84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>fresta</t>
   </si>
   <si>
     <t>chartn</t>
@@ -1049,6 +1046,10 @@
   </si>
   <si>
     <t>index_en</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>fresta_en</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1446,7 +1447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1471,7 +1472,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1479,7 +1480,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -1487,7 +1488,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1501,7 +1502,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1521,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0FC8B8-3740-45D4-A5FA-75052BCDA48C}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="B15" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="19.5" x14ac:dyDescent="0.2"/>
@@ -1536,10 +1537,10 @@
   <sheetData>
     <row r="1" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s" ph="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1547,7 +1548,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1555,7 +1556,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1563,7 +1564,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1571,7 +1572,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -1585,13 +1586,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C7" t="s" ph="1">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s" ph="1">
         <v>6</v>
-      </c>
-      <c r="D7" t="s" ph="1">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
@@ -1599,13 +1600,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
@@ -1613,21 +1614,21 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C9" t="s" ph="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
@@ -1635,13 +1636,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C11" t="s" ph="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1649,40 +1650,40 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C12" t="s" ph="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C14" t="s" ph="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1690,13 +1691,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C16" t="s" ph="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1704,13 +1705,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C17" t="s" ph="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1718,21 +1719,21 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C18" t="s" ph="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52" ph="1" x14ac:dyDescent="0.2">
@@ -1740,13 +1741,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C20" t="s" ph="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1754,21 +1755,21 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C21" t="s" ph="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
@@ -1776,13 +1777,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C23" t="s" ph="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="65" ph="1" x14ac:dyDescent="0.2">
@@ -1790,13 +1791,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C24" t="s" ph="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1804,13 +1805,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C25" t="s" ph="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -1824,8 +1825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1838,10 +1839,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1849,7 +1850,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1857,7 +1858,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1865,7 +1866,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -1873,7 +1874,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1887,13 +1888,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="182" x14ac:dyDescent="0.2">
@@ -1901,13 +1902,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -1915,13 +1916,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -1929,13 +1930,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1950,7 +1951,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1963,10 +1964,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1974,7 +1975,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1982,7 +1983,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1990,12 +1991,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2003,13 +2004,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -2017,13 +2018,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2031,13 +2032,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2045,13 +2046,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2059,13 +2060,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2073,13 +2074,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2087,21 +2088,21 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -2115,13 +2116,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2134,8 +2135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2148,10 +2149,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2159,7 +2160,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2167,7 +2168,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2175,7 +2176,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2183,7 +2184,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2194,7 +2195,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2202,13 +2203,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2216,13 +2217,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>47</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2230,13 +2231,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2244,13 +2245,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2258,18 +2259,18 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>51</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2277,13 +2278,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2291,13 +2292,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
         <v>54</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2305,13 +2306,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2319,13 +2320,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>57</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2333,13 +2334,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2347,13 +2348,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2367,8 +2368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2381,10 +2382,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2392,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2400,7 +2401,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2408,7 +2409,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -2416,7 +2417,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2427,7 +2428,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="156" x14ac:dyDescent="0.2">
@@ -2435,18 +2436,18 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2454,37 +2455,37 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2492,13 +2493,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2506,18 +2507,18 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
         <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2525,21 +2526,21 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2547,13 +2548,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2561,13 +2562,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2575,13 +2576,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2589,13 +2590,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2603,13 +2604,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2623,8 +2624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2637,10 +2638,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2648,7 +2649,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2656,7 +2657,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2664,7 +2665,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="208" x14ac:dyDescent="0.2">
@@ -2672,7 +2673,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2683,7 +2684,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2705,13 +2706,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>63</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2719,18 +2720,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>65</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2752,13 +2753,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>68</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2766,13 +2767,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>70</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2780,13 +2781,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2794,13 +2795,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2808,13 +2809,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>73</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2822,13 +2823,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" t="s">
         <v>75</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>76</v>
-      </c>
-      <c r="D18" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2836,13 +2837,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2850,13 +2851,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2864,18 +2865,18 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
         <v>80</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2897,13 +2898,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
         <v>83</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2911,13 +2912,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2925,18 +2926,18 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>86</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -2958,13 +2959,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
         <v>89</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2972,13 +2973,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
         <v>91</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2986,13 +2987,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
         <v>93</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3000,13 +3001,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3014,13 +3015,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
         <v>96</v>
-      </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="195" x14ac:dyDescent="0.2">
@@ -3028,13 +3029,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3042,13 +3043,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3056,13 +3057,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3070,13 +3071,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3084,26 +3085,26 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
         <v>198</v>
-      </c>
-      <c r="C38" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3111,7 +3112,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -3125,13 +3126,13 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3139,13 +3140,13 @@
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
         <v>101</v>
-      </c>
-      <c r="C43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -3153,21 +3154,21 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" t="s">
         <v>103</v>
-      </c>
-      <c r="C44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3175,13 +3176,13 @@
         <v>4</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" t="s">
         <v>105</v>
-      </c>
-      <c r="C46" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -3212,7 +3213,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3220,7 +3221,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3228,7 +3229,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3236,7 +3237,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -3247,7 +3248,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="260" x14ac:dyDescent="0.2">
@@ -3255,7 +3256,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -3266,7 +3267,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -3274,7 +3275,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
fix some form error in win10_en
</commit_message>
<xml_diff>
--- a/win10_en.xlsx
+++ b/win10_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{1E479151-A472-4CB0-AAF7-C7ED08DEE80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E75A4FA4-27EF-49CC-B7B9-E03B1F97E37C}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{1E479151-A472-4CB0-AAF7-C7ED08DEE80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A03F9507-E01B-4D25-9F9A-CA4D21DE644E}"/>
   <bookViews>
-    <workbookView xWindow="8992" yWindow="1200" windowWidth="16216" windowHeight="13590" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="1148" windowWidth="17205" windowHeight="14159" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="241">
   <si>
     <t>header1</t>
   </si>
@@ -991,9 +991,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>fresta</t>
-  </si>
-  <si>
     <t>moodle-login.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1010,7 +1007,84 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Let us login to the learning management system "HIRODAI moodle"
+    <t>&lt;strong&gt;You need your HIRODAI ID(student ID) and HIRODAI Password to go on this chapter.&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>Follow the link to access "HIRODAI moodle".
+&lt;a href="https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/"&gt;https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/&lt;/a&gt;
+Click "Login by HIRODAI ID"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Input HIRODAI ID(your student number) to the "User Name" box, and input your HIRODAI password to the "Password" box.
+ (*) This login form may be skipped. This is a normal behavier, so please go on.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirm that you can see a page similar to this pic.&lt;span class="check"&gt;check-8&lt;/span&gt;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h2&gt;&lt;a name="mfa"&gt;&lt;/a&gt;setup multi-factor authentication(MFA)&lt;/h2&gt; </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "How to setup MFA" in "HIRODAI moodle", and read the instruction in the course.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Follow the instruction to setup MFA of your IMC account.&lt;span class="check"&gt;check-9&lt;/span&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Follow the instruction to setup MFA of your HIRODAI ID.&lt;span class="check"&gt;check-10&lt;/span&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"HIRODAI moodle", and setup MFA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2022 Win10en chap.5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Run &amp;quot;Excel&amp;quot; in your PC.
+&lt;p class="spl"&gt; * If you cannot run &amp;quot;Excel&amp;quot; for now, you have to download Office to your PC. You can sign in to Office 365 on the Web, and install your Office desktop apps from the top page of your Office 365. See chapter 5. &lt;/p&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2022 Win10en chap.6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2022 Win10en conclusion</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Submit the Laptop checklist&lt;/h2&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Submit the Laptop checklist: Helpdesk information </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Follor this link HIRODAI moodle to login by your HIRODAI ID.
+&lt;a href="https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/"&gt;https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/&lt;/a&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Submit the Laptop checklist.&lt;/strong&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Login to the LMS "HIRODAI moodle", and setup multi-factor authentication(MFA) of your IMC account and HIRODAI ID.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Let us login to the learning management system "HIRODAI moodle" and setup MFA.
  &lt;ul&gt;
 &lt;li&gt;&lt;a href="#moodle"&gt;login to "HIRODAI moodle"&lt;/a&gt;
 &lt;/li&gt;
@@ -1020,84 +1094,15 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;strong&gt;You need your HIRODAI ID(student ID) and HIRODAI Password to go on this chapter.&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>Follow the link to access "HIRODAI moodle".
-&lt;a href="https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/"&gt;https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/&lt;/a&gt;
-Click "Login by HIRODAI ID"</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Input HIRODAI ID(your student number) to the "User Name" box, and input your HIRODAI password to the "Password" box.
- (*) This login form may be skipped. This is a normal behavier, so please go on.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Confirm that you can see a page similar to this pic.&lt;span class="check"&gt;check-8&lt;/span&gt;
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h2&gt;&lt;a name="mfa"&gt;&lt;/a&gt;setup multi-factor authentication(MFA)&lt;/h2&gt; </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Click "How to setup MFA" in "HIRODAI moodle", and read the instruction in the course.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Follow the instruction to setup MFA of your IMC account.&lt;span class="check"&gt;check-9&lt;/span&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Follow the instruction to setup MFA of your HIRODAI ID.&lt;span class="check"&gt;check-10&lt;/span&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>"HIRODAI moodle", and setup MFA</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Login to the LMS "HIRODAI moodle", and setup multi-factor authentication(MFA) of your IMC account and HIRODAI ID</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2022 Win10en chap.5</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Run &amp;quot;Excel&amp;quot; in your PC.
-&lt;p class="spl"&gt; * If you cannot run &amp;quot;Excel&amp;quot; for now, you have to download Office to your PC. You can sign in to Office 365 on the Web, and install your Office desktop apps from the top page of your Office 365. See chapter 5. &lt;/p&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2022 Win10en chap.6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2022 Win10en conclusion</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;If you have finished to set/check your PC with Chapter 1 to &lt;it&gt;here&lt;/it&gt; of this startup instruction, let&amp;apos;s open the HIRODAI moodle course &amp;quot;Laptop checklist 2022&amp;quot;, and submit the checklist!&lt;/strong&gt; </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Submit the Laptop checklist&lt;/h2&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Submit the Laptop checklist: Helpdesk information </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Follor this link HIRODAI moodle to login by your HIRODAI ID.
-&lt;a href="https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/"&gt;https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/&lt;/a&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;strong&gt;Submit the Laptop checklist.&lt;/strong&gt;</t>
+    <t xml:space="preserve">&lt;h2&gt;&lt;a name="moodle"&gt;&lt;/a&gt;login to "HIRODAI moodle"(MFA)&lt;/h2&gt; </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If you have finished to set/check your PC with Chapter 1 to &lt;it&gt;here&lt;/it&gt; of this startup instruction, let&amp;apos;s open the HIRODAI moodle course &amp;quot;Laptop checklist 2022&amp;quot;, and submit the checklist.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Now you can finish this workshop by submitting the Laptop checklist from HIRODAI moodle!&lt;/strong&gt; Also, here is helpdesk information.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2226,8 +2231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2384,7 +2389,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -2480,10 +2485,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575F79BE-20B6-421E-8137-BA7093D36AA2}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2499,7 +2504,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2507,7 +2512,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2515,7 +2520,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>215</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2523,7 +2528,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2534,7 +2539,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>220</v>
+        <v>237</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2550,59 +2555,53 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D9" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2610,7 +2609,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -2621,9 +2620,20 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2637,8 +2647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2678,7 +2688,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="204" x14ac:dyDescent="0.25">
@@ -3173,8 +3183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3214,7 +3224,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -3356,10 +3366,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3375,7 +3385,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3399,65 +3409,70 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D7" t="s">
-        <v>162</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
+      </c>
+      <c r="D9" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
       <c r="B10" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Office365 app installation procedure in win10_en.
</commit_message>
<xml_diff>
--- a/win10_en.xlsx
+++ b/win10_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20383"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{1E479151-A472-4CB0-AAF7-C7ED08DEE80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB7D3227-8B57-41E0-823D-8F70996A32A3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41E91B7-DB44-4C5D-9BD2-94D3A1513547}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="1148" windowWidth="17205" windowHeight="14159" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3516" yWindow="1152" windowWidth="17208" windowHeight="14160" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="ch5" sheetId="7" r:id="rId7"/>
     <sheet name="ch6" sheetId="5" r:id="rId8"/>
     <sheet name="ch7" sheetId="8" r:id="rId9"/>
+    <sheet name="ch8" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="254">
   <si>
     <t>header1</t>
   </si>
@@ -488,15 +489,6 @@
 &lt;/li&gt;
  &lt;/ul&gt;
  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;You need your HIRODAI ID(student ID) and HIRODAI Password to go on this chapter.&lt;/strong&gt;
-Again, you need to remember that there are two IDs to use information services provided by Hiroshima University. These IDs are based on student number.
-One of them is called HIRODAI ID, which looks same to student number. The other is &amp;quot;IMC account&amp;quot;, which looks little bit different from student number. The first letter of student number is capital, whereas that of &amp;quot;IMC account&amp;quot; is in lowercase.
-Both IDs share password. It is called &amp;quot;HIRODAI password&amp;quot;. You will know it when you get your ID card.
-Adding &amp;quot;@hiroshima-u.ac.jp&amp;quot; behind your &amp;quot;IMC account&amp;quot;, you will get your email address as a student in Hiroshima University. The email address is called &amp;quot;HIRODAI mail address&amp;quot;. Teachers or staffs in Hiroshima University may send emails to the email address. Check your email box frequently. You will learn how to check it in Chapter 5.
-  </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1055,10 +1047,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>FRESTA-TEXT-2022 Win10en conclusion</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;h2&gt;Submit the Laptop checklist&lt;/h2&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1099,6 +1087,71 @@
   </si>
   <si>
     <t>&lt;strong&gt;Now you can finish this workshop by submitting the Laptop checklist from HIRODAI moodle!&lt;/strong&gt; Also, here is helpdesk information.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;You need your HIRODAI ID(student ID) and HIRODAI Password to go on this chapter.&lt;/strong&gt;
+Again, you need to remember that there are two IDs to use information services provided by Hiroshima University. These IDs are based on student number.
+One of them is called HIRODAI ID, which looks same to student number. The other is &amp;quot;IMC account&amp;quot;, which looks little bit different from student number. The first letter of student number is capital, whereas that of &amp;quot;IMC account&amp;quot; is in lowercase.
+Both IDs share password. It is called &amp;quot;HIRODAI password&amp;quot;. You will know it when you get your ID card.
+Adding &amp;quot;@hiroshima-u.ac.jp&amp;quot; behind your &amp;quot;IMC account&amp;quot;, you will get your email address as a student in Hiroshima University. The email address is called &amp;quot;HIRODAI mail address&amp;quot;. Teachers or staffs in Hiroshima University may send emails to the email address. Check your email box frequently. You will learn how to check it in the Appendix.
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2022 Win10en chap.7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Appendix: How to install Office365 application.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2021 Win11en chap.8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If your PC does not have preinstalled Office365, you can download it from your Office365 web page.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Please visit a web page &lt;a href="https://www.media.hiroshima-u.ac.jp/services/webmail-portal/" target="_blank" rel="noreferrer"&gt;https://www.media.hiroshima-u.ac.jp/services/webmail-portal/&lt;/a&gt; in the media center, there is a link (a waterblue button) to &lt;a href="https://portal.office.com/" target="_blank"&gt;https://portal.office.com/&lt;/a&gt;. Please visit.there.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-imc-office365-portal.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Please enter your IMC account with "@hiroshima-u.ac.jp", and password.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-ms-signin2.png</t>
+  </si>
+  <si>
+    <t>Edge would ask for the permission to store your password, please choose "never". But you can cache your sign in status by "Yes" to "Stay signed in".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-ms-signin3.png</t>
+  </si>
+  <si>
+    <t>You can find "Install Office" button on the upper right. Please click it to expand its submenu, and check "Office 365 apps". You can download the network installer onto your PC.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-office365-download.png</t>
+  </si>
+  <si>
+    <t>When you start the installer, it would ask you to confirm your decition to change your computer. After checking that the verified publisher is Microsoft, please click "Yes" to proceed the installation.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-office365-install.png</t>
+  </si>
+  <si>
+    <t>The installation itself is finished, but it is not activated yet. Please back to the chaper "Activate your Office365 app."</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1500,7 +1553,7 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -1508,7 +1561,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1516,29 +1569,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
@@ -1546,12 +1599,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1564,6 +1617,111 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{095373DC-8152-4AB8-B0FD-F0060F5FB81D}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D10" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1575,24 +1733,24 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="19.149999999999999" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1" phonetic="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1" phonetic="1"/>
     <col min="4" max="4" width="20.6640625" customWidth="1" phonetic="1"/>
-    <col min="5" max="16384" width="8.796875" phonetic="1"/>
+    <col min="5" max="16384" width="8.77734375" phonetic="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="51" ph="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s" ph="1">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s" ph="1">
         <v>0</v>
       </c>
@@ -1600,23 +1758,23 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s" ph="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ph="1" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s" ph="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ph="1" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s" ph="1">
         <v>4</v>
       </c>
@@ -1628,26 +1786,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>5</v>
@@ -1656,167 +1814,167 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D9" t="s" ph="1">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D10" t="s" ph="1">
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D10" t="s" ph="1">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D11" t="s" ph="1">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D13" t="s" ph="1">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D14" t="s" ph="1">
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D14" t="s" ph="1">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ph="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D18" t="s" ph="1">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="D18" t="s" ph="1">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="51" ph="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s" ph="1">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D21" t="s" ph="1">
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>5</v>
@@ -1825,32 +1983,32 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="63.75" ph="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ph="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1868,7 +2026,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -1876,7 +2034,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1884,7 +2042,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1892,42 +2050,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -1936,7 +2094,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1950,7 +2108,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1964,7 +2122,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1993,7 +2151,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -2001,7 +2159,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2009,7 +2167,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2017,33 +2175,33 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="102" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -2052,12 +2210,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2071,7 +2229,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2085,7 +2243,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2099,12 +2257,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -2113,7 +2271,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -2127,12 +2285,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -2146,7 +2304,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2160,12 +2318,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -2174,7 +2332,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2188,7 +2346,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -2202,12 +2360,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="102" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -2231,7 +2389,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -2239,7 +2397,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2247,7 +2405,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2255,23 +2413,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2285,83 +2443,83 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="153" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="158.4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>114</v>
+        <v>238</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" t="s">
         <v>115</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" t="s">
+    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -2375,81 +2533,81 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D18" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D18" t="s">
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -2458,18 +2616,18 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2487,7 +2645,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" customWidth="1"/>
@@ -2495,47 +2653,47 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2544,90 +2702,90 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="D10" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -2647,7 +2805,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -2655,7 +2813,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2663,7 +2821,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2671,28 +2829,28 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="204" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="211.2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2701,12 +2859,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2720,7 +2878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2734,7 +2892,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2748,12 +2906,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2767,7 +2925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -2781,21 +2939,21 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -2806,24 +2964,24 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -2837,12 +2995,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -2851,12 +3009,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -2865,7 +3023,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -2879,12 +3037,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -2898,7 +3056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -2912,12 +3070,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -2926,7 +3084,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -2940,12 +3098,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -2959,12 +3117,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -2973,7 +3131,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -2987,7 +3145,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -3001,7 +3159,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -3012,10 +3170,10 @@
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -3029,12 +3187,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="178.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -3043,68 +3201,68 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="1" t="s">
+    <row r="36" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
         <v>146</v>
       </c>
-      <c r="C37" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -3118,7 +3276,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -3132,7 +3290,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -3146,15 +3304,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="102" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -3183,7 +3341,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -3191,7 +3349,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -3199,7 +3357,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3207,28 +3365,28 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -3242,7 +3400,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -3256,7 +3414,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -3270,12 +3428,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -3284,7 +3442,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -3298,7 +3456,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -3312,7 +3470,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -3326,7 +3484,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -3340,7 +3498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="178.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -3364,11 +3522,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -3376,15 +3534,15 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3392,51 +3550,51 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="D9" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -3450,17 +3608,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="198" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
change Bb9 access win10en
</commit_message>
<xml_diff>
--- a/win10_en.xlsx
+++ b/win10_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{303C47D1-7A13-4708-995C-F605F665DAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{528B2DDB-D70A-47A9-8428-C9DF491DE445}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="13_ncr:1_{303C47D1-7A13-4708-995C-F605F665DAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F6818D5-FEE6-421B-BCA9-56143F11DB26}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="-15450" windowWidth="18225" windowHeight="11880" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3600" yWindow="-15450" windowWidth="18225" windowHeight="11880" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="260">
   <si>
     <t>header1</t>
   </si>
@@ -258,9 +258,6 @@
   </si>
   <si>
     <t>win10-6-09.svg</t>
-  </si>
-  <si>
-    <t>win10-6-11.svg</t>
   </si>
   <si>
     <t>win10-6-12.svg</t>
@@ -1085,15 +1082,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Let us try to go to a Bb9 study course from My MOMIJI. 
-Click the course link "Introduction to University Education"("大学教育入門") in the time table.
-(*) Screenshot here is under construction.</t>
-    <rPh sb="118" eb="124">
-      <t>ダイガクキョウイクニュウモン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;h2&gt;Helpdesk&lt;/h2&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1168,6 +1156,32 @@
     <t xml:space="preserve">Web Mail page will be opened. You may read HIRODAI Mails here. Since the university sends messages to your HIRODAI Mail, check the mail box frequently. &lt;span class="check"&gt;check-11&lt;/span&gt;
 You can use Outlook app to receive and send your HIRODAI Mails on your smartphone. We recommend it for daily use, as it is easy to use and it also have push notification function.
 &lt;img alt="*outlook icon*" src="image/win10-outlook-app.png" width="64" /&gt;  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-6-11a.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mymomiji-topintro.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Let us try to go to a Bb9 study course from My MOMIJI. 
+Click the course link "Introduction to University Education"("大学教育入門") in the time table.
+</t>
+    <rPh sb="118" eb="124">
+      <t>ダイガクキョウイクニュウモン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Click the link "to Bb9"("Bb9へ") .
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mymomiji-intro.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1590,7 +1604,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1598,7 +1612,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -1606,7 +1620,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1620,7 +1634,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1657,7 +1671,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1665,7 +1679,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1673,7 +1687,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1681,7 +1695,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -1689,18 +1703,18 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D7" t="s">
         <v>200</v>
-      </c>
-      <c r="D7" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -1708,31 +1722,31 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D8" t="s">
         <v>202</v>
-      </c>
-      <c r="D8" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D9" t="s">
         <v>204</v>
-      </c>
-      <c r="D9" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D10" t="s">
         <v>206</v>
-      </c>
-      <c r="D10" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -1764,7 +1778,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -1772,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -1780,7 +1794,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -1788,12 +1802,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:4" ph="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -1801,7 +1815,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s" ph="1">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>4</v>
@@ -1815,13 +1829,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -1829,13 +1843,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -1843,21 +1857,21 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -1865,24 +1879,24 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:4" ph="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -1890,21 +1904,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -1912,13 +1926,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -1926,13 +1940,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -1940,21 +1954,21 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="51" ph="1" x14ac:dyDescent="0.25">
@@ -1962,13 +1976,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -1976,21 +1990,21 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -1998,13 +2012,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="63.75" ph="1" x14ac:dyDescent="0.25">
@@ -2012,13 +2026,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -2026,13 +2040,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2063,7 +2077,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2079,7 +2093,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2087,7 +2101,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -2095,7 +2109,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2109,7 +2123,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -2123,7 +2137,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -2151,7 +2165,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2204,7 +2218,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2212,12 +2226,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -2225,7 +2239,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -2286,13 +2300,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -2319,13 +2333,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2347,7 +2361,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -2375,13 +2389,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -2389,13 +2403,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2426,7 +2440,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2442,7 +2456,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2450,7 +2464,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
@@ -2458,7 +2472,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2477,13 +2491,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2496,37 +2510,37 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2534,13 +2548,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -2559,7 +2573,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2567,13 +2581,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2581,21 +2595,21 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
         <v>218</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2603,13 +2617,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2617,13 +2631,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2631,13 +2645,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -2645,13 +2659,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -2659,13 +2673,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2696,7 +2710,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2704,7 +2718,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2712,7 +2726,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2720,7 +2734,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2731,7 +2745,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2747,20 +2761,20 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2768,13 +2782,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2782,18 +2796,18 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2801,7 +2815,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -2812,7 +2826,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -2823,7 +2837,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -2837,10 +2851,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="B27" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2856,7 +2870,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2872,7 +2886,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2880,7 +2894,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="204" x14ac:dyDescent="0.25">
@@ -2888,7 +2902,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2941,7 +2955,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2982,13 +2996,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2996,13 +3010,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -3010,13 +3024,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -3030,7 +3044,7 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -3038,7 +3052,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -3052,7 +3066,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -3077,7 +3091,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3099,29 +3113,29 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -3129,143 +3143,140 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>255</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>243</v>
+        <v>257</v>
+      </c>
+      <c r="D27" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
       <c r="B28" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D28" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
+    </row>
+    <row r="31" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
+    <row r="35" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="1" t="s">
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
         <v>66</v>
       </c>
-      <c r="C34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
+    </row>
+    <row r="36" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="1" t="s">
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
         <v>68</v>
       </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
+    </row>
+    <row r="37" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -3276,76 +3287,90 @@
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C41" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="C42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>
       </c>
       <c r="D43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" t="s" ph="1">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="102" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D44" t="s" ph="1">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="102" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="1" t="s">
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" t="s">
         <v>77</v>
-      </c>
-      <c r="C45" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -3359,8 +3384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3392,7 +3417,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3400,12 +3425,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -3413,7 +3438,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -3427,7 +3452,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -3455,7 +3480,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -3497,7 +3522,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -3531,7 +3556,7 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -3561,7 +3586,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3569,7 +3594,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3577,7 +3602,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3585,35 +3610,35 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3629,7 +3654,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
@@ -3637,7 +3662,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
fix webmail banner pics
</commit_message>
<xml_diff>
--- a/win10_en.xlsx
+++ b/win10_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="13_ncr:1_{303C47D1-7A13-4708-995C-F605F665DAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A0EECBB-F4EF-4598-9864-5A27120746C9}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="13_ncr:1_{303C47D1-7A13-4708-995C-F605F665DAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08DCA009-302F-4CB1-B7E6-0E6E4EC30DBB}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="-16050" windowWidth="21600" windowHeight="11595" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6030" yWindow="-15765" windowWidth="21600" windowHeight="11595" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -234,9 +234,6 @@
   </t>
   </si>
   <si>
-    <t>win10-6-03.svg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Office 365 applications are listed. Click &amp;quot;Outlook&amp;quot;.
   </t>
   </si>
@@ -1205,6 +1202,10 @@
 &lt;ul&gt; &lt;/ul&gt;
 &lt;/ul&gt;
 </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>momiji-webmail.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1627,7 +1628,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1635,7 +1636,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -1643,7 +1644,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1657,7 +1658,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1694,7 +1695,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1702,7 +1703,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1710,7 +1711,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1718,7 +1719,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -1726,18 +1727,18 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" t="s">
         <v>186</v>
-      </c>
-      <c r="D7" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -1745,31 +1746,31 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" t="s">
         <v>188</v>
-      </c>
-      <c r="D8" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D9" t="s">
         <v>190</v>
-      </c>
-      <c r="D9" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" t="s">
         <v>192</v>
-      </c>
-      <c r="D10" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -1801,7 +1802,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -1809,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -1817,7 +1818,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -1825,12 +1826,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:4" ph="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -1838,7 +1839,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s" ph="1">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>4</v>
@@ -1852,13 +1853,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -1866,13 +1867,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -1880,21 +1881,21 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -1902,24 +1903,24 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:4" ph="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -1927,21 +1928,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -1949,13 +1950,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -1963,13 +1964,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -1977,21 +1978,21 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="51" ph="1" x14ac:dyDescent="0.25">
@@ -1999,13 +2000,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -2013,21 +2014,21 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -2035,13 +2036,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="63.75" ph="1" x14ac:dyDescent="0.25">
@@ -2049,13 +2050,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -2063,13 +2064,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2100,7 +2101,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2116,7 +2117,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2124,7 +2125,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -2132,7 +2133,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2146,7 +2147,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -2160,7 +2161,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -2188,7 +2189,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2241,7 +2242,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2249,12 +2250,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -2262,7 +2263,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -2323,13 +2324,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -2356,13 +2357,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2384,7 +2385,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -2412,13 +2413,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -2426,13 +2427,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2463,7 +2464,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2479,7 +2480,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2487,7 +2488,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
@@ -2495,7 +2496,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2514,13 +2515,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2533,37 +2534,37 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2571,13 +2572,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -2596,7 +2597,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2604,13 +2605,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2618,21 +2619,21 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
         <v>204</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2640,13 +2641,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2654,13 +2655,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2668,13 +2669,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -2682,13 +2683,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -2696,13 +2697,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2733,7 +2734,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2741,7 +2742,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2749,7 +2750,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2757,7 +2758,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2768,7 +2769,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2784,7 +2785,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2825,18 +2826,18 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2844,29 +2845,29 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2874,13 +2875,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2888,18 +2889,18 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2907,21 +2908,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -2929,21 +2930,21 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -2951,13 +2952,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -2970,8 +2971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="B26" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B26" sqref="A26:XFD32"/>
+    <sheetView tabSelected="1" topLeftCell="C18" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2987,7 +2988,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3003,7 +3004,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3011,7 +3012,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="204" x14ac:dyDescent="0.25">
@@ -3019,7 +3020,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3052,13 +3053,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3091,7 +3092,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3099,13 +3100,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -3113,13 +3114,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -3127,13 +3128,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -3141,13 +3142,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -3155,13 +3156,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -3169,13 +3170,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -3183,18 +3184,18 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>60</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3216,29 +3217,29 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -3246,34 +3247,34 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D28" t="s">
         <v>236</v>
-      </c>
-      <c r="D28" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -3281,18 +3282,18 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -3300,13 +3301,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -3314,18 +3315,18 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -3333,7 +3334,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -3347,13 +3348,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
@@ -3361,21 +3362,21 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -3383,13 +3384,13 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3436,7 +3437,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3444,12 +3445,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -3457,7 +3458,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -3471,7 +3472,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -3499,7 +3500,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -3541,7 +3542,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -3575,7 +3576,7 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3588,8 +3589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3605,7 +3606,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3613,7 +3614,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3621,7 +3622,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3629,35 +3630,35 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3673,7 +3674,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
@@ -3681,7 +3682,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
remove Bb9 mentions from English texts
</commit_message>
<xml_diff>
--- a/win10_en.xlsx
+++ b/win10_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D4EE04-B038-4E76-9A81-0D85596AC5DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E7AC42-CB37-44E8-A1F5-B0CD7161A2BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6708" yWindow="-15096" windowWidth="21600" windowHeight="11592" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6708" yWindow="-15096" windowWidth="21600" windowHeight="11592" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -747,10 +747,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Office365, My MOMIJI, Bb9, and others…</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;strong&gt;(*) If you have purchased your Windows PC at Hiroshima University Co-op, please follow the initial setup instrucrion from the shop, and start this workshop from chapter 1.&lt;/strong&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -922,16 +918,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>momiji-bb9moodle.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>lms-moodle.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Click the banner "Bb9/moodle" at right side.
-  </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -999,30 +986,6 @@
 You can find more information on &lt;a href="https://www.media.hiroshima-u.ac.jp/services/hinet/vpngw"&gt;IMC web site&lt;/a&gt;
 . 
   </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Let us start from the MOMIJI top page again.
-You can see many banners on the right of the page. In this chapter, we will explain &amp;quot;Web Mail&amp;quot;, &amp;quot;My MOMIJI&amp;quot; and &amp;quot;Bb9&amp;quot;.
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Let us log in to the online services provided by university, such as My MOMIJI, Office365, or Bb9.
-You need a browser to use these services. Microsoft Edge has already been in Windows10. Then double-click its icon to open it.
-&lt;ul&gt;&lt;li&gt;&lt;a href="#momiji"&gt;MOMIJI: Student Portal&lt;/a&gt;
-&lt;/li&gt;
-&lt;li&gt;&lt;a href="#mail"&gt;Office365: Web mail service and online storage&lt;/a&gt;
-&lt;/li&gt;
-&lt;li&gt;&lt;a href="#mymomiji"&gt;My MOMIJI: Class enrollment, bulletin board etc.&lt;/a&gt;
-&lt;/li&gt;
-&lt;li&gt;&lt;a href="#bb9"&gt;Bb9: Learning management system&lt;/a&gt;
-&lt;/li&gt;
-&lt;li&gt;&lt;a href="#omake"&gt;Others&lt;/a&gt;
-&lt;/li&gt;
-&lt;ul&gt; &lt;/ul&gt;
-&lt;/ul&gt;
-</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1257,6 +1220,37 @@
     <t xml:space="preserve">When you are asked to continue connecting, click &amp;quot;Connect&amp;quot;. 
 When your PC has successfully connected to the Wi-Fi, you will see the word &amp;quot;Connected&amp;quot; under the name of the Wi-Fi. &lt;span class="check"&gt;check-14&lt;/span&gt;
    </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Click the banner "Moodle" at right side.
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Office365, My MOMIJI, and others…</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>momiji-moodle.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Let us log in to the online services provided by university, such as My MOMIJI, Office365.
+You need a browser to use these services. Microsoft Edge has already been in Windows10. Then double-click its icon to open it.
+&lt;ul&gt;
+&lt;li&gt;&lt;a href="#momiji"&gt;MOMIJI: Student Portal&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#mail"&gt;Office365: Web mail service and online storage&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#mymomiji"&gt;My MOMIJI: Class enrollment, bulletin board etc.&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#omake"&gt;Others&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Let us start from the MOMIJI top page again.
+You can see many banners on the right of the page. In this chapter, we will explain &amp;quot;Web Mail&amp;quot;, &amp;quot;My MOMIJI&amp;quot;.
+  </t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1690,7 +1684,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -1698,7 +1692,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1880,12 +1874,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
@@ -1893,7 +1887,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s" ph="1">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>4</v>
@@ -2179,7 +2173,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -2215,7 +2209,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -2304,12 +2298,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -2378,7 +2372,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -2439,7 +2433,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -2481,7 +2475,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -2492,7 +2486,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2500,76 +2494,76 @@
     </row>
     <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D25" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D26" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D27" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D28" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D29" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D30" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D31" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D32" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -2577,7 +2571,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
@@ -2585,47 +2579,47 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D37" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D39" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D40" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D41" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D42" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2680,7 +2674,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -2688,7 +2682,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2707,7 +2701,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -2726,7 +2720,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2797,7 +2791,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -2811,18 +2805,18 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
         <v>180</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D19" t="s">
         <v>96</v>
@@ -2889,7 +2883,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -2909,8 +2903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575F79BE-20B6-421E-8137-BA7093D36AA2}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="C14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2926,7 +2920,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2934,7 +2928,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2950,7 +2944,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2961,7 +2955,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2977,7 +2971,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3018,18 +3012,18 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3037,26 +3031,26 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>211</v>
+        <v>275</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>209</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D16" t="s">
         <v>153</v>
@@ -3067,7 +3061,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -3081,13 +3075,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -3100,21 +3094,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D21" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3122,21 +3116,21 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D23" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3144,18 +3138,19 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3163,8 +3158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -3180,7 +3175,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>174</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3204,15 +3199,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="211.2" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="132" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>226</v>
+        <v>278</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3245,13 +3240,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>225</v>
+        <v>279</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3284,7 +3279,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3306,7 +3301,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -3340,7 +3335,7 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -3348,7 +3343,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -3387,7 +3382,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -3409,18 +3404,18 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D23" t="s">
         <v>154</v>
@@ -3428,7 +3423,7 @@
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D24" t="s">
         <v>172</v>
@@ -3439,13 +3434,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -3508,7 +3503,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
@@ -3517,7 +3512,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="D38" ph="1"/>
     </row>
   </sheetData>
@@ -3531,8 +3526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -3572,7 +3567,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3585,7 +3580,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -3624,7 +3619,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -3666,7 +3661,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -3694,7 +3689,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -3755,12 +3750,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3770,12 +3765,12 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D9" t="s">
         <v>153</v>
@@ -3783,10 +3778,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D10" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3802,7 +3797,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="198" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win10en: fix check number
</commit_message>
<xml_diff>
--- a/win10_en.xlsx
+++ b/win10_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20407"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BB1B03-D90E-4EC1-BF41-B2FEE32DBEA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63885FB9-9F73-4743-BD96-2F2D5383B0F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6708" yWindow="-15096" windowWidth="21600" windowHeight="11592" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6708" yWindow="-15096" windowWidth="21600" windowHeight="11592" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -737,11 +737,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">Confirm that you can see "Dashboard" similar to this pic.&lt;span class="check"&gt;check-8&lt;/span&gt;
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;strong&gt;You need your Hirodai ID(student ID) and Hirodai Password to go on this chapter.&lt;/strong&gt;</t>
   </si>
   <si>
@@ -915,18 +910,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Click "MFA configuration guide", and you can see the top page of "MFA21" course.Please read comment sheet.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Click "IMCアカウントのMFA設定" below.</t>
     <rPh sb="19" eb="21">
       <t>セッテイ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Click "Practice setting up MFA use of IMC accounts" below, and follow instruction to setup MFA. See PDF documents for details.&lt;span class="check"&gt;check-9&lt;/span&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -952,11 +939,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">Click "Practice setting up MFA use of Hirodai ID" below, and follow instruction to setup MFA. See PDF documents for details.&lt;span class="check"&gt;check-10&lt;/span&gt;
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>moodle-checklist.svg</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1155,12 +1137,6 @@
     <t xml:space="preserve">Click &amp;quot;I agree&amp;quot;.
 Now you can use Microsoft Office applications!&lt;span class="check"&gt;check-12&lt;/span&gt;
 </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">When you are asked to continue connecting, click &amp;quot;Connect&amp;quot;. 
-When your PC has successfully connected to the Wi-Fi, you will see the word &amp;quot;Connected&amp;quot; under the name of the Wi-Fi. &lt;span class="check"&gt;check-14&lt;/span&gt;
-   </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1252,6 +1228,30 @@
 You can find more information on &lt;a href="https://www.media.hiroshima-u.ac.jp/services/print/webprint"&gt;IMC web site&lt;/a&gt;
 . It&amp;apos;s Japanese only. Please check Google translation menu at the bottom of right column.
   </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirm that you can see "Dashboard" similar to this pic.&lt;span class="check"&gt;check-7&lt;/span&gt;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Practice setting up MFA use of IMC accounts" below, and follow instruction to setup MFA. See PDF documents for details.&lt;span class="check"&gt;check-8&lt;/span&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "MFA configuration guide", and you can see the top page of "MFA21" course. Please read comment sheet.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Click "Practice setting up MFA use of Hirodai ID" below, and follow instruction to setup MFA. See PDF documents for details.&lt;span class="check"&gt;check-9&lt;/span&gt;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">When you are asked to continue connecting, click &amp;quot;Connect&amp;quot;. 
+When your PC has successfully connected to the Wi-Fi, you will see the word &amp;quot;Connected&amp;quot; under the name of the Wi-Fi. &lt;span class="check"&gt;check-13&lt;/span&gt;
+   </t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1685,7 +1685,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -1693,7 +1693,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1875,7 +1875,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -2174,7 +2174,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -2210,7 +2210,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -2258,7 +2258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4804C742-A9A0-451E-9571-F0E1882D4FEC}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -2299,7 +2299,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -2373,7 +2373,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -2434,7 +2434,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -2476,7 +2476,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -2487,7 +2487,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2495,76 +2495,76 @@
     </row>
     <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D25" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D26" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D27" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D28" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D29" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D30" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D31" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D32" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -2572,7 +2572,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
@@ -2580,47 +2580,47 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D37" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D39" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D40" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D41" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D42" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2634,8 +2634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2675,7 +2675,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -2683,7 +2683,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2702,13 +2702,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2817,7 +2817,7 @@
     </row>
     <row r="19" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D19" t="s">
         <v>87</v>
@@ -2884,7 +2884,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -2905,7 +2905,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView topLeftCell="B16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2921,7 +2921,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2929,7 +2929,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2945,7 +2945,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2956,7 +2956,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2972,7 +2972,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3013,18 +3013,18 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3032,26 +3032,26 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D16" t="s">
         <v>143</v>
@@ -3062,7 +3062,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -3076,13 +3076,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>171</v>
+        <v>274</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -3095,21 +3095,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>207</v>
+        <v>276</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3117,21 +3117,21 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>209</v>
+        <v>275</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3139,13 +3139,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>213</v>
+        <v>277</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3159,8 +3159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C24" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="B17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -3176,7 +3176,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3200,7 +3200,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -3208,7 +3208,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3241,13 +3241,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3280,7 +3280,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3302,7 +3302,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -3336,7 +3336,7 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -3344,7 +3344,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -3372,7 +3372,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -3383,7 +3383,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -3405,18 +3405,18 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D23" t="s">
         <v>144</v>
@@ -3424,7 +3424,7 @@
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D24" t="s">
         <v>162</v>
@@ -3435,13 +3435,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -3468,7 +3468,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
@@ -3501,7 +3501,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
@@ -3524,8 +3524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -3565,7 +3565,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3578,7 +3578,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -3595,7 +3595,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -3617,13 +3617,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -3637,7 +3637,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -3651,7 +3651,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -3659,13 +3659,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -3687,13 +3687,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -3748,12 +3748,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3763,12 +3763,12 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D9" t="s">
         <v>143</v>
@@ -3776,10 +3776,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D10" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3795,7 +3795,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="198" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win10_en.xlsx: note about EOL of Windows10.
</commit_message>
<xml_diff>
--- a/win10_en.xlsx
+++ b/win10_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9888322B-BE9C-4999-BB83-751A935D4AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216ABB1E-B83B-4FB9-9A6D-A67225407B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -460,12 +460,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">You are going to prepare your PC for your study life at Hiroshima University during this lecture. Here is the list of what you are going to do at this workshop.
-&lt;ol&gt; &lt;/ol&gt;
-* Some screenshots in this text are displayed in Japanese. Sorry for inconvenience. </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Microsoft Teams will run automatically. Click x at right up in the window to close the application for now.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1228,6 +1222,15 @@
 &lt;li&gt;&lt;a href="#mfa-imc-account"&gt;setup multi-factor authentication (MFA) for IMC account&lt;/a&gt;
 &lt;/li&gt;
  &lt;/ul&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;strong&gt;
+Microsoft announces that the support of Windows 10 would be terminated on 2025-Oct-25. The connection of the outdated operating systems to the campus network is seriously discouraged. You can initialize your PC by Windows 10 for now, but you should migrate to Windows 11 as soon as possible. 
+&lt;/strong&gt;
+You are going to prepare your PC for your study life at Hiroshima University during this lecture. Here is the list of what you are going to do at this workshop.
+&lt;ol&gt; &lt;/ol&gt;
+* Some screenshots in this text are displayed in Japanese. Sorry for inconvenience. &lt;&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1597,19 +1600,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="100.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="4" max="4" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1617,29 +1620,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>234</v>
-      </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
@@ -1647,12 +1650,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="148.5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>105</v>
+        <v>274</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1676,95 +1679,95 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="100.6328125" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="100.625" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B5" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B7" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
+      <c r="D7" t="s">
         <v>151</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" t="s">
         <v>153</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="B9" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+      <c r="D9" t="s">
         <v>155</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="B10" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+      <c r="D10" t="s">
         <v>157</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B11" s="1" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1782,24 +1785,24 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="19.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="21" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1" phonetic="1"/>
-    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1" phonetic="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1" phonetic="1"/>
-    <col min="5" max="16384" width="8.81640625" phonetic="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1" phonetic="1"/>
+    <col min="2" max="2" width="100.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1" phonetic="1"/>
+    <col min="4" max="4" width="20.625" customWidth="1" phonetic="1"/>
+    <col min="5" max="16384" width="8.875" phonetic="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="65" ph="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="67.5" ph="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s" ph="1">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s" ph="1">
         <v>0</v>
       </c>
@@ -1807,33 +1810,33 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s" ph="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ph="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s" ph="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ph="1" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="42" ph="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s" ph="1">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>4</v>
@@ -1842,7 +1845,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="40.5" ph="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s" ph="1">
         <v>4</v>
       </c>
@@ -1853,10 +1856,10 @@
         <v>5</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="27" ph="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s" ph="1">
         <v>4</v>
       </c>
@@ -1870,7 +1873,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="27" ph="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s" ph="1">
         <v>4</v>
       </c>
@@ -1881,18 +1884,18 @@
         <v>5</v>
       </c>
       <c r="D10" t="s" ph="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="27" ph="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" t="s" ph="1">
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" t="s" ph="1">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="27" ph="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s" ph="1">
         <v>4</v>
       </c>
@@ -1903,21 +1906,21 @@
         <v>5</v>
       </c>
       <c r="D12" t="s" ph="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ph="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="1" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="40.5" ph="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s" ph="1">
         <v>4</v>
       </c>
@@ -1928,18 +1931,18 @@
         <v>5</v>
       </c>
       <c r="D14" t="s" ph="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="27" ph="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" t="s" ph="1">
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D15" t="s" ph="1">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ph="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s" ph="1">
         <v>4</v>
       </c>
@@ -1950,46 +1953,46 @@
         <v>5</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="40.5" ph="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="27" ph="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
         <v>100</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="52" ph="1" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="54" ph="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s" ph="1">
         <v>4</v>
       </c>
@@ -2000,10 +2003,10 @@
         <v>5</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="27" ph="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s" ph="1">
         <v>4</v>
       </c>
@@ -2014,10 +2017,10 @@
         <v>5</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="27" ph="1" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
         <v>103</v>
       </c>
@@ -2025,7 +2028,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="26" ph="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="27" ph="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s" ph="1">
         <v>4</v>
       </c>
@@ -2039,26 +2042,26 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="65" ph="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="67.5" ph="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>5</v>
@@ -2082,15 +2085,15 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="100.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="4" max="4" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2098,7 +2101,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2106,42 +2109,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="108" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="81" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="78" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -2150,12 +2153,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="143" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="148.5" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -2164,7 +2167,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="78" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="81" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2178,7 +2181,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="143" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="148.5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2207,15 +2210,15 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="100.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="4" max="4" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2223,7 +2226,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2231,28 +2234,28 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="108" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2266,12 +2269,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2285,7 +2288,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2299,7 +2302,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2313,12 +2316,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="78" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="81" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -2327,7 +2330,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -2341,12 +2344,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -2360,7 +2363,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2374,12 +2377,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -2388,7 +2391,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="81" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2402,7 +2405,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="78" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="81" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -2416,12 +2419,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -2430,142 +2433,142 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B22" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="B24" s="3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" ht="65" x14ac:dyDescent="0.2">
-      <c r="B24" s="3" t="s">
+    <row r="25" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+      <c r="B25" s="3" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
+      <c r="D25" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+      <c r="B26" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="65" x14ac:dyDescent="0.2">
-      <c r="B26" s="3" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B27" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="3" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B28" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="3" t="s">
+    <row r="29" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="B29" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="B29" s="3" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B30" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D30" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="B31" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="D29" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="3" t="s">
+      <c r="D31" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="B32" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="D30" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="B31" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="B32" s="3" t="s">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B33" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="D32" t="s">
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B35" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B37" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D37" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="3" t="s">
+    <row r="38" spans="2:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="B38" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="D37" t="s">
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B39" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D39" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="B38" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="3" t="s">
+    <row r="40" spans="2:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="B40" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="40" spans="2:4" ht="39" x14ac:dyDescent="0.2">
-      <c r="B40" s="3" t="s">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B41" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="3" t="s">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B42" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D42" t="s">
-        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2583,15 +2586,15 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="100.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="4" max="4" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2599,7 +2602,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2607,28 +2610,28 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="117" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="121.5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2637,36 +2640,36 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="156" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="162" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2675,7 +2678,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
         <v>79</v>
       </c>
@@ -2683,7 +2686,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
         <v>82</v>
       </c>
@@ -2691,7 +2694,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
         <v>83</v>
       </c>
@@ -2699,7 +2702,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2713,7 +2716,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -2727,17 +2730,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -2746,43 +2749,43 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
         <v>168</v>
       </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -2793,24 +2796,24 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -2824,12 +2827,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -2849,59 +2852,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575F79BE-20B6-421E-8137-BA7093D36AA2}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B11" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="100.6328125" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="100.625" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="4" max="4" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="156" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="148.5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2910,22 +2913,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2939,7 +2942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2953,116 +2956,116 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B13" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+      <c r="B15" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D15" t="s">
         <v>194</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B16" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D15" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
         <v>197</v>
       </c>
-      <c r="D16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B20" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="3" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="D21" s="4" t="s">
+    </row>
+    <row r="22" spans="1:4" s="4" customFormat="1" ht="12.95" customHeight="1" ph="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="4" customFormat="1" ht="13" customHeight="1" ph="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="3" t="s">
+    <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="3" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>272</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -3080,23 +3083,23 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="100.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="4" max="4" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3104,28 +3107,28 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="130" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="135" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3134,12 +3137,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -3153,26 +3156,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -3186,7 +3189,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -3197,52 +3200,52 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -3253,15 +3256,15 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="78" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="81" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -3270,7 +3273,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -3284,12 +3287,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -3298,12 +3301,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -3317,56 +3320,56 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="B23" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="39" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="D23" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D24" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -3380,18 +3383,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="117" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="121.5" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -3405,7 +3408,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
         <v>70</v>
       </c>
@@ -3413,12 +3416,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
@@ -3427,7 +3430,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="4:4" ht="19.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:4" ht="21" x14ac:dyDescent="0.15">
       <c r="D38" ph="1"/>
     </row>
   </sheetData>
@@ -3445,15 +3448,15 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="100.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="4" max="4" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -3461,7 +3464,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3469,39 +3472,39 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="143" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="148.5" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -3512,10 +3515,10 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -3529,21 +3532,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -3554,10 +3557,10 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="81" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -3568,24 +3571,24 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="65" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -3599,18 +3602,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="182" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="189" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -3628,23 +3631,23 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="100.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="4" max="4" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3652,75 +3655,75 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B7" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="B8" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="B9" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+      <c r="D9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B10" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B12" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D10" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="195" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:4" ht="202.5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>

</xml_diff>